<commit_message>
Update NashVille-Fried-Software - MS1-P2-A.xlsx
</commit_message>
<xml_diff>
--- a/NashVille-Fried-Software - MS1-P2-A.xlsx
+++ b/NashVille-Fried-Software - MS1-P2-A.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="177">
   <si>
     <t>Team Name</t>
   </si>
@@ -543,13 +543,16 @@
   </si>
   <si>
     <t>Conversation Link</t>
+  </si>
+  <si>
+    <t>https://chatgpt.com/share/67f7b229-28f0-8004-998d-e5172ee63804</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -630,6 +633,12 @@
     <font>
       <b/>
       <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -892,7 +901,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -992,6 +1001,9 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="13" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
@@ -8434,31 +8446,33 @@
       <c r="A3" s="37">
         <v>1.0</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="38" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="37">
         <v>2.0</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="39"/>
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="37">
         <v>3.0</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="39"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="37">
         <v>4.0</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="A7" s="37">
         <v>5.0</v>
       </c>
-      <c r="B7" s="38"/>
+      <c r="B7" s="39"/>
     </row>
     <row r="8" ht="12.0" customHeight="1"/>
     <row r="9" ht="12.0" customHeight="1"/>
@@ -9457,9 +9471,12 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B3"/>
+  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>